<commit_message>
removes email from inst docs
</commit_message>
<xml_diff>
--- a/inst/extdata/Banet-Example/metadata/data-package-metadata.xlsx
+++ b/inst/extdata/Banet-Example/metadata/data-package-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA_Salmonid_Habitat_Monitoring\data-raw\mandy-salmanid-habitat-monitoring\Enclosure Study - Growth Rates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\EMLaide\inst\extdata\Banet-Example\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C599064-0CED-427F-A36B-D6C9F1E8F880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B275F1-EAD8-4C8A-BB3B-5CE0AD4D635B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26220" yWindow="-14385" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10080" yWindow="-16560" windowWidth="29040" windowHeight="15840" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="141">
   <si>
     <t>first_name</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Banet</t>
   </si>
   <si>
-    <t>abanet@csuchico edu</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
@@ -267,12 +264,6 @@
   </si>
   <si>
     <t>Greathouse</t>
-  </si>
-  <si>
-    <t>sptussing@earthlink.net</t>
-  </si>
-  <si>
-    <t>rgreathouse@psmfc.org</t>
   </si>
   <si>
     <t>Tussing Ecological Services</t>
@@ -465,6 +456,9 @@
   </si>
   <si>
     <t>R14AC00096</t>
+  </si>
+  <si>
+    <t>mail@mail.mail</t>
   </si>
 </sst>
 </file>
@@ -1053,12 +1047,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1145,20 +1139,20 @@
     </row>
     <row r="2" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1171,20 +1165,20 @@
     </row>
     <row r="3" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1197,29 +1191,29 @@
     </row>
     <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="12"/>
@@ -1233,29 +1227,29 @@
     </row>
     <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="12"/>
@@ -1269,29 +1263,29 @@
     </row>
     <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
@@ -1305,29 +1299,29 @@
     </row>
     <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="12"/>
@@ -1341,29 +1335,29 @@
     </row>
     <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="12"/>
@@ -1377,29 +1371,29 @@
     </row>
     <row r="9" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="12"/>
@@ -1413,29 +1407,29 @@
     </row>
     <row r="10" spans="1:14" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="12"/>
@@ -1449,29 +1443,29 @@
     </row>
     <row r="11" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="12"/>
@@ -1485,29 +1479,29 @@
     </row>
     <row r="12" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="12"/>
@@ -1521,20 +1515,20 @@
     </row>
     <row r="13" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -1547,20 +1541,20 @@
     </row>
     <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1573,29 +1567,29 @@
     </row>
     <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="12"/>
@@ -53030,8 +53024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -53070,70 +53064,70 @@
         <v>65</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>72</v>
+      <c r="E4" t="s">
+        <v>76</v>
       </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>78</v>
+      <c r="C5" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -53145,10 +53139,8 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A37CF2EA-0AA4-7A48-A3BB-03E5CF2F125C}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{D8E80961-D1A2-5244-B87D-840FC2B1161C}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{E9A54F23-8915-6B43-97BC-C66A57BFB9D2}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{2AC411AF-987A-B149-A8A4-5DE2C0DC111F}"/>
-    <hyperlink ref="F2" r:id="rId5" xr:uid="{B6FD44FE-5996-BC4C-BC30-CA815CE3CCC8}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{B6FD44FE-5996-BC4C-BC30-CA815CE3CCC8}"/>
+    <hyperlink ref="C3:C5" r:id="rId3" display="mail@mail.mail" xr:uid="{DACC7E74-28B9-4FB6-9873-501385EA217E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -53179,10 +53171,10 @@
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -53215,27 +53207,27 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -53279,7 +53271,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -53337,25 +53329,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -53376,7 +53368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -53412,14 +53404,14 @@
     </row>
     <row r="2" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -53459,10 +53451,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -53526,7 +53518,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1">
         <v>-122.448217</v>

</xml_diff>

<commit_message>
Edits new create-EML-from-template and restrucutres pkgdown site, rebuilds site
</commit_message>
<xml_diff>
--- a/inst/extdata/Banet-Example/metadata/data-package-metadata.xlsx
+++ b/inst/extdata/Banet-Example/metadata/data-package-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\EMLaide\inst\extdata\Banet-Example\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B275F1-EAD8-4C8A-BB3B-5CE0AD4D635B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C45619-BEA4-43DF-B2C2-DFCCCDA5AB36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10080" yWindow="-16560" windowWidth="29040" windowHeight="15840" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53025,7 +53025,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>